<commit_message>
annotating affirmative yes values in code book
</commit_message>
<xml_diff>
--- a/data/nov/[9800] Amplify AAPI M3 November 2023 - Codebook.xlsx
+++ b/data/nov/[9800] Amplify AAPI M3 November 2023 - Codebook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\NPPC\Common\AmeriSpeak\ClientServices\Projects\Amplify AAPI\9800 Month 3 - November 2023\Data\Main\A4S\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vpeng/git/norc/data/nov/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B332F351-737F-4436-9D92-65889754C419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F04CB3-A812-4D46-9B0E-75B72E7BC0AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13550" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0BE2CFA7-70CD-48B7-AD55-013317C63E6A}"/>
+    <workbookView xWindow="1560" yWindow="1640" windowWidth="30220" windowHeight="18300" xr2:uid="{0BE2CFA7-70CD-48B7-AD55-013317C63E6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Codebook" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="5">
   <si>
     <t>Variable</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Value Label</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -4235,21 +4238,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F95F401F-6B65-4A90-BABC-8BDD054269B9}">
-  <dimension ref="A1:D356"/>
+  <dimension ref="A1:E356"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.28515625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="61.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="61.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4263,7 +4266,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>'[1]PASTE Variable Val in A1'!A3</f>
         <v>SAMPLE_SOURCE</v>
@@ -4281,7 +4284,7 @@
         <v>Amerispeak</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C3" s="4">
         <f>'[1]PASTE Variable Val in A1'!B4</f>
         <v>2</v>
@@ -4291,7 +4294,7 @@
         <v>Amplify AAPI</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f>'[1]PASTE Variable Val in A1'!A5</f>
         <v>Q1A</v>
@@ -4308,8 +4311,11 @@
         <f>'[1]PASTE Variable Val in A1'!C5</f>
         <v>Often true</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C5" s="4">
         <f>'[1]PASTE Variable Val in A1'!B6</f>
         <v>2</v>
@@ -4318,8 +4324,11 @@
         <f>'[1]PASTE Variable Val in A1'!C6</f>
         <v>Sometimes true</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C6" s="4">
         <f>'[1]PASTE Variable Val in A1'!B7</f>
         <v>3</v>
@@ -4329,7 +4338,7 @@
         <v>Never true</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C7" s="4">
         <f>'[1]PASTE Variable Val in A1'!B8</f>
         <v>77</v>
@@ -4339,7 +4348,7 @@
         <v>Don't know</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C8" s="4">
         <f>'[1]PASTE Variable Val in A1'!B9</f>
         <v>98</v>
@@ -4349,7 +4358,7 @@
         <v>SKIPPED ON WEB</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C9" s="4">
         <f>'[1]PASTE Variable Val in A1'!B10</f>
         <v>99</v>
@@ -4359,7 +4368,7 @@
         <v>Refused</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f>'[1]PASTE Variable Val in A1'!A11</f>
         <v>Q1B</v>
@@ -4376,8 +4385,11 @@
         <f>'[1]PASTE Variable Val in A1'!C11</f>
         <v>Often true</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C11" s="4">
         <f>'[1]PASTE Variable Val in A1'!B12</f>
         <v>2</v>
@@ -4386,8 +4398,11 @@
         <f>'[1]PASTE Variable Val in A1'!C12</f>
         <v>Sometimes true</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C12" s="4">
         <f>'[1]PASTE Variable Val in A1'!B13</f>
         <v>3</v>
@@ -4397,7 +4412,7 @@
         <v>Never true</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C13" s="4">
         <f>'[1]PASTE Variable Val in A1'!B14</f>
         <v>77</v>
@@ -4407,7 +4422,7 @@
         <v>Don't know</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C14" s="4">
         <f>'[1]PASTE Variable Val in A1'!B15</f>
         <v>98</v>
@@ -4417,7 +4432,7 @@
         <v>SKIPPED ON WEB</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C15" s="4">
         <f>'[1]PASTE Variable Val in A1'!B16</f>
         <v>99</v>
@@ -4427,7 +4442,7 @@
         <v>Refused</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
         <f>'[1]PASTE Variable Val in A1'!A17</f>
         <v>Q3</v>
@@ -4444,8 +4459,11 @@
         <f>'[1]PASTE Variable Val in A1'!C17</f>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C17" s="4">
         <f>'[1]PASTE Variable Val in A1'!B18</f>
         <v>2</v>
@@ -4455,7 +4473,7 @@
         <v>No</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C18" s="4">
         <f>'[1]PASTE Variable Val in A1'!B19</f>
         <v>77</v>
@@ -4465,7 +4483,7 @@
         <v>Don't know</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C19" s="4">
         <f>'[1]PASTE Variable Val in A1'!B20</f>
         <v>98</v>
@@ -4475,7 +4493,7 @@
         <v>SKIPPED ON WEB</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C20" s="4">
         <f>'[1]PASTE Variable Val in A1'!B21</f>
         <v>99</v>
@@ -4485,7 +4503,7 @@
         <v>REFUSED</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
         <f>'[1]PASTE Variable Val in A1'!A22</f>
         <v>Q4</v>
@@ -4502,8 +4520,11 @@
         <f>'[1]PASTE Variable Val in A1'!C22</f>
         <v>Almost every month</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C22" s="4">
         <f>'[1]PASTE Variable Val in A1'!B23</f>
         <v>2</v>
@@ -4512,8 +4533,11 @@
         <f>'[1]PASTE Variable Val in A1'!C23</f>
         <v>Some months but not every month</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C23" s="4">
         <f>'[1]PASTE Variable Val in A1'!B24</f>
         <v>3</v>
@@ -4523,7 +4547,7 @@
         <v>Only 1 or 2 months</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C24" s="4">
         <f>'[1]PASTE Variable Val in A1'!B25</f>
         <v>77</v>
@@ -4533,7 +4557,7 @@
         <v>Don't know</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C25" s="4">
         <f>'[1]PASTE Variable Val in A1'!B26</f>
         <v>98</v>
@@ -4543,7 +4567,7 @@
         <v>SKIPPED ON WEB</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C26" s="4">
         <f>'[1]PASTE Variable Val in A1'!B27</f>
         <v>99</v>
@@ -4553,7 +4577,7 @@
         <v>REFUSED</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" t="str">
         <f>'[1]PASTE Variable Val in A1'!A28</f>
         <v>Q5</v>
@@ -4570,8 +4594,11 @@
         <f>'[1]PASTE Variable Val in A1'!C28</f>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C28" s="4">
         <f>'[1]PASTE Variable Val in A1'!B29</f>
         <v>2</v>
@@ -4581,7 +4608,7 @@
         <v>No</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C29" s="4">
         <f>'[1]PASTE Variable Val in A1'!B30</f>
         <v>77</v>
@@ -4591,7 +4618,7 @@
         <v>Don't know</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C30" s="4">
         <f>'[1]PASTE Variable Val in A1'!B31</f>
         <v>98</v>
@@ -4601,7 +4628,7 @@
         <v>SKIPPED ON WEB</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C31" s="4">
         <f>'[1]PASTE Variable Val in A1'!B32</f>
         <v>99</v>
@@ -4611,7 +4638,7 @@
         <v>REFUSED</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" t="str">
         <f>'[1]PASTE Variable Val in A1'!A33</f>
         <v>Q6</v>
@@ -4628,8 +4655,11 @@
         <f>'[1]PASTE Variable Val in A1'!C33</f>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C33" s="4">
         <f>'[1]PASTE Variable Val in A1'!B34</f>
         <v>2</v>
@@ -4639,7 +4669,7 @@
         <v>No</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C34" s="4">
         <f>'[1]PASTE Variable Val in A1'!B35</f>
         <v>77</v>
@@ -4649,7 +4679,7 @@
         <v>Don't know</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C35" s="4">
         <f>'[1]PASTE Variable Val in A1'!B36</f>
         <v>98</v>
@@ -4659,7 +4689,7 @@
         <v>SKIPPED ON WEB</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C36" s="4">
         <f>'[1]PASTE Variable Val in A1'!B37</f>
         <v>99</v>
@@ -4669,7 +4699,7 @@
         <v>REFUSED</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" t="str">
         <f>'[1]PASTE Variable Val in A1'!A38</f>
         <v>Q7</v>
@@ -4687,7 +4717,7 @@
         <v>Very hard</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C38" s="4">
         <f>'[1]PASTE Variable Val in A1'!B39</f>
         <v>2</v>
@@ -4697,7 +4727,7 @@
         <v>Hard</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C39" s="4">
         <f>'[1]PASTE Variable Val in A1'!B40</f>
         <v>3</v>
@@ -4707,7 +4737,7 @@
         <v>Somewhat hard</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C40" s="4">
         <f>'[1]PASTE Variable Val in A1'!B41</f>
         <v>4</v>
@@ -4717,7 +4747,7 @@
         <v>Not very hard</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C41" s="4">
         <f>'[1]PASTE Variable Val in A1'!B42</f>
         <v>5</v>
@@ -4727,7 +4757,7 @@
         <v>Not hard at all</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C42" s="4">
         <f>'[1]PASTE Variable Val in A1'!B43</f>
         <v>77</v>
@@ -4737,7 +4767,7 @@
         <v>Don't know</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C43" s="4">
         <f>'[1]PASTE Variable Val in A1'!B44</f>
         <v>98</v>
@@ -4747,7 +4777,7 @@
         <v>SKIPPED ON WEB</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C44" s="4">
         <f>'[1]PASTE Variable Val in A1'!B45</f>
         <v>99</v>
@@ -4757,7 +4787,7 @@
         <v>Refused</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A45" t="str">
         <f>'[1]PASTE Variable Val in A1'!A46</f>
         <v>Q8A</v>
@@ -4775,7 +4805,7 @@
         <v>Often true</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C46" s="4">
         <f>'[1]PASTE Variable Val in A1'!B47</f>
         <v>2</v>
@@ -4785,7 +4815,7 @@
         <v>Sometimes true</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C47" s="4">
         <f>'[1]PASTE Variable Val in A1'!B48</f>
         <v>3</v>
@@ -4795,7 +4825,7 @@
         <v>Never true</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C48" s="4">
         <f>'[1]PASTE Variable Val in A1'!B49</f>
         <v>77</v>
@@ -4805,7 +4835,7 @@
         <v>DON'T KNOW</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C49" s="4">
         <f>'[1]PASTE Variable Val in A1'!B50</f>
         <v>98</v>
@@ -4815,7 +4845,7 @@
         <v>SKIPPED ON WEB</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C50" s="4">
         <f>'[1]PASTE Variable Val in A1'!B51</f>
         <v>99</v>
@@ -4825,7 +4855,7 @@
         <v>REFUSED</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A51" t="str">
         <f>'[1]PASTE Variable Val in A1'!A52</f>
         <v>Q8B</v>
@@ -4843,7 +4873,7 @@
         <v>Often true</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C52" s="4">
         <f>'[1]PASTE Variable Val in A1'!B53</f>
         <v>2</v>
@@ -4853,7 +4883,7 @@
         <v>Sometimes true</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C53" s="4">
         <f>'[1]PASTE Variable Val in A1'!B54</f>
         <v>3</v>
@@ -4863,7 +4893,7 @@
         <v>Never true</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C54" s="4">
         <f>'[1]PASTE Variable Val in A1'!B55</f>
         <v>77</v>
@@ -4873,7 +4903,7 @@
         <v>DON'T KNOW</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C55" s="4">
         <f>'[1]PASTE Variable Val in A1'!B56</f>
         <v>98</v>
@@ -4883,7 +4913,7 @@
         <v>SKIPPED ON WEB</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C56" s="4">
         <f>'[1]PASTE Variable Val in A1'!B57</f>
         <v>99</v>
@@ -4893,7 +4923,7 @@
         <v>REFUSED</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A57" t="str">
         <f>'[1]PASTE Variable Val in A1'!A58</f>
         <v>Q8C</v>
@@ -4911,7 +4941,7 @@
         <v>Often true</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C58" s="4">
         <f>'[1]PASTE Variable Val in A1'!B59</f>
         <v>2</v>
@@ -4921,7 +4951,7 @@
         <v>Sometimes true</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C59" s="4">
         <f>'[1]PASTE Variable Val in A1'!B60</f>
         <v>3</v>
@@ -4931,7 +4961,7 @@
         <v>Never true</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C60" s="4">
         <f>'[1]PASTE Variable Val in A1'!B61</f>
         <v>77</v>
@@ -4941,7 +4971,7 @@
         <v>DON'T KNOW</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C61" s="4">
         <f>'[1]PASTE Variable Val in A1'!B62</f>
         <v>98</v>
@@ -4951,7 +4981,7 @@
         <v>SKIPPED ON WEB</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C62" s="4">
         <f>'[1]PASTE Variable Val in A1'!B63</f>
         <v>99</v>
@@ -4961,7 +4991,7 @@
         <v>REFUSED</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A63" t="str">
         <f>'[1]PASTE Variable Val in A1'!A64</f>
         <v>Q8D</v>
@@ -4979,7 +5009,7 @@
         <v>Often true</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C64" s="4">
         <f>'[1]PASTE Variable Val in A1'!B65</f>
         <v>2</v>
@@ -4989,7 +5019,7 @@
         <v>Sometimes true</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C65" s="4">
         <f>'[1]PASTE Variable Val in A1'!B66</f>
         <v>3</v>
@@ -4999,7 +5029,7 @@
         <v>Never true</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C66" s="4">
         <f>'[1]PASTE Variable Val in A1'!B67</f>
         <v>77</v>
@@ -5009,7 +5039,7 @@
         <v>DON'T KNOW</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C67" s="4">
         <f>'[1]PASTE Variable Val in A1'!B68</f>
         <v>98</v>
@@ -5019,7 +5049,7 @@
         <v>SKIPPED ON WEB</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C68" s="4">
         <f>'[1]PASTE Variable Val in A1'!B69</f>
         <v>99</v>
@@ -5029,7 +5059,7 @@
         <v>REFUSED</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A69" t="str">
         <f>'[1]PASTE Variable Val in A1'!A70</f>
         <v>Q8E</v>
@@ -5047,7 +5077,7 @@
         <v>Often true</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C70" s="4">
         <f>'[1]PASTE Variable Val in A1'!B71</f>
         <v>2</v>
@@ -5057,7 +5087,7 @@
         <v>Sometimes true</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C71" s="4">
         <f>'[1]PASTE Variable Val in A1'!B72</f>
         <v>3</v>
@@ -5067,7 +5097,7 @@
         <v>Never true</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C72" s="4">
         <f>'[1]PASTE Variable Val in A1'!B73</f>
         <v>77</v>
@@ -5077,7 +5107,7 @@
         <v>DON'T KNOW</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C73" s="4">
         <f>'[1]PASTE Variable Val in A1'!B74</f>
         <v>98</v>
@@ -5087,7 +5117,7 @@
         <v>SKIPPED ON WEB</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C74" s="4">
         <f>'[1]PASTE Variable Val in A1'!B75</f>
         <v>99</v>
@@ -5097,7 +5127,7 @@
         <v>REFUSED</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A75" t="str">
         <f>'[1]PASTE Variable Val in A1'!A76</f>
         <v>Q8F</v>
@@ -5115,7 +5145,7 @@
         <v>Often true</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C76" s="4">
         <f>'[1]PASTE Variable Val in A1'!B77</f>
         <v>2</v>
@@ -5125,7 +5155,7 @@
         <v>Sometimes true</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C77" s="4">
         <f>'[1]PASTE Variable Val in A1'!B78</f>
         <v>3</v>
@@ -5135,7 +5165,7 @@
         <v>Never true</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C78" s="4">
         <f>'[1]PASTE Variable Val in A1'!B79</f>
         <v>77</v>
@@ -5145,7 +5175,7 @@
         <v>DON'T KNOW</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C79" s="4">
         <f>'[1]PASTE Variable Val in A1'!B80</f>
         <v>98</v>
@@ -5155,7 +5185,7 @@
         <v>SKIPPED ON WEB</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C80" s="4">
         <f>'[1]PASTE Variable Val in A1'!B81</f>
         <v>99</v>
@@ -5165,7 +5195,7 @@
         <v>REFUSED</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A81" t="str">
         <f>'[1]PASTE Variable Val in A1'!A82</f>
         <v>Q8G</v>
@@ -5183,7 +5213,7 @@
         <v>Often true</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C82" s="4">
         <f>'[1]PASTE Variable Val in A1'!B83</f>
         <v>2</v>
@@ -5193,7 +5223,7 @@
         <v>Sometimes true</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C83" s="4">
         <f>'[1]PASTE Variable Val in A1'!B84</f>
         <v>3</v>
@@ -5203,7 +5233,7 @@
         <v>Never true</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C84" s="4">
         <f>'[1]PASTE Variable Val in A1'!B85</f>
         <v>77</v>
@@ -5213,7 +5243,7 @@
         <v>DON'T KNOW</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C85" s="4">
         <f>'[1]PASTE Variable Val in A1'!B86</f>
         <v>98</v>
@@ -5223,7 +5253,7 @@
         <v>SKIPPED ON WEB</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C86" s="4">
         <f>'[1]PASTE Variable Val in A1'!B87</f>
         <v>99</v>
@@ -5233,7 +5263,7 @@
         <v>REFUSED</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A87" t="str">
         <f>'[1]PASTE Variable Val in A1'!A88</f>
         <v>Q8H</v>
@@ -5251,7 +5281,7 @@
         <v>Often true</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C88" s="4">
         <f>'[1]PASTE Variable Val in A1'!B89</f>
         <v>2</v>
@@ -5261,7 +5291,7 @@
         <v>Sometimes true</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C89" s="4">
         <f>'[1]PASTE Variable Val in A1'!B90</f>
         <v>3</v>
@@ -5271,7 +5301,7 @@
         <v>Never true</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C90" s="4">
         <f>'[1]PASTE Variable Val in A1'!B91</f>
         <v>77</v>
@@ -5281,7 +5311,7 @@
         <v>DON'T KNOW</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C91" s="4">
         <f>'[1]PASTE Variable Val in A1'!B92</f>
         <v>98</v>
@@ -5291,7 +5321,7 @@
         <v>SKIPPED ON WEB</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C92" s="4">
         <f>'[1]PASTE Variable Val in A1'!B93</f>
         <v>99</v>
@@ -5301,7 +5331,7 @@
         <v>REFUSED</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A93" t="str">
         <f>'[1]PASTE Variable Val in A1'!A94</f>
         <v>Q8I</v>
@@ -5319,7 +5349,7 @@
         <v>Often true</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C94" s="4">
         <f>'[1]PASTE Variable Val in A1'!B95</f>
         <v>2</v>
@@ -5329,7 +5359,7 @@
         <v>Sometimes true</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C95" s="4">
         <f>'[1]PASTE Variable Val in A1'!B96</f>
         <v>3</v>
@@ -5339,7 +5369,7 @@
         <v>Never true</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C96" s="4">
         <f>'[1]PASTE Variable Val in A1'!B97</f>
         <v>77</v>
@@ -5349,7 +5379,7 @@
         <v>DON'T KNOW</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C97" s="4">
         <f>'[1]PASTE Variable Val in A1'!B98</f>
         <v>98</v>
@@ -5359,7 +5389,7 @@
         <v>SKIPPED ON WEB</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C98" s="4">
         <f>'[1]PASTE Variable Val in A1'!B99</f>
         <v>99</v>
@@ -5369,7 +5399,7 @@
         <v>REFUSED</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A99" t="str">
         <f>'[1]PASTE Variable Val in A1'!A100</f>
         <v>Q8J</v>
@@ -5387,7 +5417,7 @@
         <v>Often true</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C100" s="4">
         <f>'[1]PASTE Variable Val in A1'!B101</f>
         <v>2</v>
@@ -5397,7 +5427,7 @@
         <v>Sometimes true</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C101" s="4">
         <f>'[1]PASTE Variable Val in A1'!B102</f>
         <v>3</v>
@@ -5407,7 +5437,7 @@
         <v>Never true</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C102" s="4">
         <f>'[1]PASTE Variable Val in A1'!B103</f>
         <v>77</v>
@@ -5417,7 +5447,7 @@
         <v>DON'T KNOW</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C103" s="4">
         <f>'[1]PASTE Variable Val in A1'!B104</f>
         <v>98</v>
@@ -5427,7 +5457,7 @@
         <v>SKIPPED ON WEB</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C104" s="4">
         <f>'[1]PASTE Variable Val in A1'!B105</f>
         <v>99</v>
@@ -5437,7 +5467,7 @@
         <v>REFUSED</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A105" t="str">
         <f>'[1]PASTE Variable Val in A1'!A106</f>
         <v>Q8K</v>
@@ -5455,7 +5485,7 @@
         <v>Often true</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C106" s="4">
         <f>'[1]PASTE Variable Val in A1'!B107</f>
         <v>2</v>
@@ -5465,7 +5495,7 @@
         <v>Sometimes true</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C107" s="4">
         <f>'[1]PASTE Variable Val in A1'!B108</f>
         <v>3</v>
@@ -5475,7 +5505,7 @@
         <v>Never true</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C108" s="4">
         <f>'[1]PASTE Variable Val in A1'!B109</f>
         <v>77</v>
@@ -5485,7 +5515,7 @@
         <v>DON'T KNOW</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C109" s="4">
         <f>'[1]PASTE Variable Val in A1'!B110</f>
         <v>98</v>
@@ -5495,7 +5525,7 @@
         <v>SKIPPED ON WEB</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C110" s="4">
         <f>'[1]PASTE Variable Val in A1'!B111</f>
         <v>99</v>
@@ -5505,7 +5535,7 @@
         <v>REFUSED</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A111" t="str">
         <f>'[1]PASTE Variable Val in A1'!A112</f>
         <v>Q8L</v>
@@ -5523,7 +5553,7 @@
         <v>Often true</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C112" s="4">
         <f>'[1]PASTE Variable Val in A1'!B113</f>
         <v>2</v>
@@ -5533,7 +5563,7 @@
         <v>Sometimes true</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C113" s="4">
         <f>'[1]PASTE Variable Val in A1'!B114</f>
         <v>3</v>
@@ -5543,7 +5573,7 @@
         <v>Never true</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C114" s="4">
         <f>'[1]PASTE Variable Val in A1'!B115</f>
         <v>77</v>
@@ -5553,7 +5583,7 @@
         <v>DON'T KNOW</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C115" s="4">
         <f>'[1]PASTE Variable Val in A1'!B116</f>
         <v>98</v>
@@ -5563,7 +5593,7 @@
         <v>SKIPPED ON WEB</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C116" s="4">
         <f>'[1]PASTE Variable Val in A1'!B117</f>
         <v>99</v>
@@ -5573,7 +5603,7 @@
         <v>REFUSED</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A117" t="str">
         <f>'[1]PASTE Variable Val in A1'!A118</f>
         <v>Q8M</v>
@@ -5591,7 +5621,7 @@
         <v>Often true</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C118" s="4">
         <f>'[1]PASTE Variable Val in A1'!B119</f>
         <v>2</v>
@@ -5601,7 +5631,7 @@
         <v>Sometimes true</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C119" s="4">
         <f>'[1]PASTE Variable Val in A1'!B120</f>
         <v>3</v>
@@ -5611,7 +5641,7 @@
         <v>Never true</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C120" s="4">
         <f>'[1]PASTE Variable Val in A1'!B121</f>
         <v>77</v>
@@ -5621,7 +5651,7 @@
         <v>DON'T KNOW</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C121" s="4">
         <f>'[1]PASTE Variable Val in A1'!B122</f>
         <v>98</v>
@@ -5631,7 +5661,7 @@
         <v>SKIPPED ON WEB</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C122" s="4">
         <f>'[1]PASTE Variable Val in A1'!B123</f>
         <v>99</v>
@@ -5641,7 +5671,7 @@
         <v>REFUSED</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A123" t="str">
         <f>'[1]PASTE Variable Val in A1'!A124</f>
         <v>Q9</v>
@@ -5659,7 +5689,7 @@
         <v>Yes, I have received SNAP benefits in the past, but I do not currently.</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C124" s="4">
         <f>'[1]PASTE Variable Val in A1'!B125</f>
         <v>2</v>
@@ -5669,7 +5699,7 @@
         <v>Yes, I am enrolled in SNAP now and currently receive benefits</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C125" s="4">
         <f>'[1]PASTE Variable Val in A1'!B126</f>
         <v>3</v>
@@ -5679,7 +5709,7 @@
         <v>No</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C126" s="4">
         <f>'[1]PASTE Variable Val in A1'!B127</f>
         <v>77</v>
@@ -5689,7 +5719,7 @@
         <v>I don't know</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C127" s="4">
         <f>'[1]PASTE Variable Val in A1'!B128</f>
         <v>98</v>
@@ -5699,7 +5729,7 @@
         <v>SKIPPED ON WEB</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C128" s="4">
         <f>'[1]PASTE Variable Val in A1'!B129</f>
         <v>99</v>
@@ -5709,7 +5739,7 @@
         <v>REFUSED</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A129" t="str">
         <f>'[1]PASTE Variable Val in A1'!A130</f>
         <v>Q10</v>
@@ -5727,7 +5757,7 @@
         <v>I don’t know if I am eligible</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C130" s="4">
         <f>'[1]PASTE Variable Val in A1'!B131</f>
         <v>2</v>
@@ -5737,7 +5767,7 @@
         <v>I am not eligible</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C131" s="4">
         <f>'[1]PASTE Variable Val in A1'!B132</f>
         <v>3</v>
@@ -5747,7 +5777,7 @@
         <v>I am not comfortable accepting help from the government for food</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C132" s="4">
         <f>'[1]PASTE Variable Val in A1'!B133</f>
         <v>4</v>
@@ -5757,7 +5787,7 @@
         <v>I do not think it’s the government’s job to pay for food</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C133" s="4">
         <f>'[1]PASTE Variable Val in A1'!B134</f>
         <v>5</v>
@@ -5767,7 +5797,7 @@
         <v>I don’t know how to sign up</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C134" s="4">
         <f>'[1]PASTE Variable Val in A1'!B135</f>
         <v>6</v>
@@ -5777,7 +5807,7 @@
         <v>The process to sign up is too difficult</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C135" s="4">
         <f>'[1]PASTE Variable Val in A1'!B136</f>
         <v>7</v>
@@ -5787,7 +5817,7 @@
         <v>I’m worried about signing up given the citizenship status of me or members of my household</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C136" s="4">
         <f>'[1]PASTE Variable Val in A1'!B137</f>
         <v>77</v>
@@ -5797,7 +5827,7 @@
         <v>DON'T KNOW</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C137" s="4">
         <f>'[1]PASTE Variable Val in A1'!B138</f>
         <v>98</v>
@@ -5807,7 +5837,7 @@
         <v>SKIPPED ON WEB</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C138" s="4">
         <f>'[1]PASTE Variable Val in A1'!B139</f>
         <v>99</v>
@@ -5817,7 +5847,7 @@
         <v>REFUSED</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A139" t="str">
         <f>'[1]PASTE Variable Val in A1'!A140</f>
         <v>duration_ROCKEFELLER</v>
@@ -5835,7 +5865,7 @@
         <v>Under 1 minute</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A140" t="str">
         <f>'[1]PASTE Variable Val in A1'!A141</f>
         <v>SURV_MODE</v>
@@ -5853,7 +5883,7 @@
         <v>Phone interview</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C141" s="4">
         <f>'[1]PASTE Variable Val in A1'!B142</f>
         <v>2</v>
@@ -5863,7 +5893,7 @@
         <v>Web Interview</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A142" t="str">
         <f>'[1]PASTE Variable Val in A1'!A143</f>
         <v>SURV_LANG</v>
@@ -5881,7 +5911,7 @@
         <v>English</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C143" s="4">
         <f>'[1]PASTE Variable Val in A1'!B144</f>
         <v>2</v>
@@ -5891,7 +5921,7 @@
         <v>Chinese Traditional</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C144" s="4">
         <f>'[1]PASTE Variable Val in A1'!B145</f>
         <v>3</v>
@@ -5901,7 +5931,7 @@
         <v>Chinese Simplified</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C145" s="4">
         <f>'[1]PASTE Variable Val in A1'!B146</f>
         <v>4</v>
@@ -5911,7 +5941,7 @@
         <v>Korean</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C146" s="4">
         <f>'[1]PASTE Variable Val in A1'!B147</f>
         <v>5</v>
@@ -5921,7 +5951,7 @@
         <v>Vietnamese</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A147" t="str">
         <f>'[1]PASTE Variable Val in A1'!A148</f>
         <v>GENDER</v>
@@ -5939,7 +5969,7 @@
         <v>Unknown</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C148" s="4">
         <f>'[1]PASTE Variable Val in A1'!B149</f>
         <v>1</v>
@@ -5949,7 +5979,7 @@
         <v>Male</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C149" s="4">
         <f>'[1]PASTE Variable Val in A1'!B150</f>
         <v>2</v>
@@ -5959,7 +5989,7 @@
         <v>Female</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A150" t="str">
         <f>'[1]PASTE Variable Val in A1'!A151</f>
         <v>AGE4</v>
@@ -5977,7 +6007,7 @@
         <v>18-29</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C151" s="4">
         <f>'[1]PASTE Variable Val in A1'!B152</f>
         <v>2</v>
@@ -5987,7 +6017,7 @@
         <v>30-44</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C152" s="4">
         <f>'[1]PASTE Variable Val in A1'!B153</f>
         <v>3</v>
@@ -5997,7 +6027,7 @@
         <v>45-59</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C153" s="4">
         <f>'[1]PASTE Variable Val in A1'!B154</f>
         <v>4</v>
@@ -6007,7 +6037,7 @@
         <v>60+</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C154" s="4">
         <f>'[1]PASTE Variable Val in A1'!B155</f>
         <v>99</v>
@@ -6017,7 +6047,7 @@
         <v>Under 18</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A155" t="str">
         <f>'[1]PASTE Variable Val in A1'!A156</f>
         <v>AGE7</v>
@@ -6035,7 +6065,7 @@
         <v>18-24</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C156" s="4">
         <f>'[1]PASTE Variable Val in A1'!B157</f>
         <v>2</v>
@@ -6045,7 +6075,7 @@
         <v>25-34</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C157" s="4">
         <f>'[1]PASTE Variable Val in A1'!B158</f>
         <v>3</v>
@@ -6055,7 +6085,7 @@
         <v>35-44</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C158" s="4">
         <f>'[1]PASTE Variable Val in A1'!B159</f>
         <v>4</v>
@@ -6065,7 +6095,7 @@
         <v>45-54</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C159" s="4">
         <f>'[1]PASTE Variable Val in A1'!B160</f>
         <v>5</v>
@@ -6075,7 +6105,7 @@
         <v>55-64</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C160" s="4">
         <f>'[1]PASTE Variable Val in A1'!B161</f>
         <v>6</v>
@@ -6085,7 +6115,7 @@
         <v>65-74</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C161" s="4">
         <f>'[1]PASTE Variable Val in A1'!B162</f>
         <v>7</v>
@@ -6095,7 +6125,7 @@
         <v>75+</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C162" s="4">
         <f>'[1]PASTE Variable Val in A1'!B163</f>
         <v>99</v>
@@ -6105,7 +6135,7 @@
         <v>Under 18</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A163" t="str">
         <f>'[1]PASTE Variable Val in A1'!A164</f>
         <v>ASIANORIGIN</v>
@@ -6123,7 +6153,7 @@
         <v>Chinese (and no other AAPI origin)</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C164" s="4">
         <f>'[1]PASTE Variable Val in A1'!B165</f>
         <v>2</v>
@@ -6133,7 +6163,7 @@
         <v>Asian Indian (and no other AAPI origin)</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C165" s="4">
         <f>'[1]PASTE Variable Val in A1'!B166</f>
         <v>3</v>
@@ -6143,7 +6173,7 @@
         <v>Filipino (and no other AAPI origin)</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C166" s="4">
         <f>'[1]PASTE Variable Val in A1'!B167</f>
         <v>4</v>
@@ -6153,7 +6183,7 @@
         <v>Vietnamese (and no other AAPI origin)</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C167" s="4">
         <f>'[1]PASTE Variable Val in A1'!B168</f>
         <v>5</v>
@@ -6163,7 +6193,7 @@
         <v>Korean (and no other AAPI origin)</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C168" s="4">
         <f>'[1]PASTE Variable Val in A1'!B169</f>
         <v>6</v>
@@ -6173,7 +6203,7 @@
         <v>Japanese (and no other AAPI origin)</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C169" s="4">
         <f>'[1]PASTE Variable Val in A1'!B170</f>
         <v>7</v>
@@ -6183,7 +6213,7 @@
         <v>Native Hawaiian/Pacific Island (and no other AAPI origin)</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C170" s="4">
         <f>'[1]PASTE Variable Val in A1'!B171</f>
         <v>8</v>
@@ -6193,7 +6223,7 @@
         <v>Other singular AAPI origin</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C171" s="4">
         <f>'[1]PASTE Variable Val in A1'!B172</f>
         <v>9</v>
@@ -6203,7 +6233,7 @@
         <v>Multiple AAPI origins</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A172" t="str">
         <f>'[1]PASTE Variable Val in A1'!A173</f>
         <v>AAPIORIGIN_CHINESE</v>
@@ -6221,7 +6251,7 @@
         <v>No</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C173" s="4">
         <f>'[1]PASTE Variable Val in A1'!B174</f>
         <v>1</v>
@@ -6231,7 +6261,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A174" t="str">
         <f>'[1]PASTE Variable Val in A1'!A175</f>
         <v>AAPIORIGIN_ASIANINDIAN</v>
@@ -6249,7 +6279,7 @@
         <v>No</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C175" s="4">
         <f>'[1]PASTE Variable Val in A1'!B176</f>
         <v>1</v>
@@ -6259,7 +6289,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A176" t="str">
         <f>'[1]PASTE Variable Val in A1'!A177</f>
         <v>AAPIORIGIN_FILIPINO</v>
@@ -6277,7 +6307,7 @@
         <v>No</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C177" s="4">
         <f>'[1]PASTE Variable Val in A1'!B178</f>
         <v>1</v>
@@ -6287,7 +6317,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A178" t="str">
         <f>'[1]PASTE Variable Val in A1'!A179</f>
         <v>AAPIORIGIN_VIETNAMESE</v>
@@ -6305,7 +6335,7 @@
         <v>No</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C179" s="4">
         <f>'[1]PASTE Variable Val in A1'!B180</f>
         <v>1</v>
@@ -6315,7 +6345,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A180" t="str">
         <f>'[1]PASTE Variable Val in A1'!A181</f>
         <v>AAPIORIGIN_KOREAN</v>
@@ -6333,7 +6363,7 @@
         <v>No</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C181" s="4">
         <f>'[1]PASTE Variable Val in A1'!B182</f>
         <v>1</v>
@@ -6343,7 +6373,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A182" t="str">
         <f>'[1]PASTE Variable Val in A1'!A183</f>
         <v>AAPIORIGIN_JAPANESE</v>
@@ -6361,7 +6391,7 @@
         <v>No</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C183" s="4">
         <f>'[1]PASTE Variable Val in A1'!B184</f>
         <v>1</v>
@@ -6371,7 +6401,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A184" t="str">
         <f>'[1]PASTE Variable Val in A1'!A185</f>
         <v>AAPIORIGIN_NATIVEHAWAIIAN</v>
@@ -6389,7 +6419,7 @@
         <v>No</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C185" s="4">
         <f>'[1]PASTE Variable Val in A1'!B186</f>
         <v>1</v>
@@ -6399,7 +6429,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A186" t="str">
         <f>'[1]PASTE Variable Val in A1'!A187</f>
         <v>AAPIORIGIN_GUAMANIANCHAMORRO</v>
@@ -6417,7 +6447,7 @@
         <v>No</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C187" s="4">
         <f>'[1]PASTE Variable Val in A1'!B188</f>
         <v>1</v>
@@ -6427,7 +6457,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A188" t="str">
         <f>'[1]PASTE Variable Val in A1'!A189</f>
         <v>AAPIORIGIN_SAMOAN</v>
@@ -6445,7 +6475,7 @@
         <v>No</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C189" s="4">
         <f>'[1]PASTE Variable Val in A1'!B190</f>
         <v>1</v>
@@ -6455,7 +6485,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A190" t="str">
         <f>'[1]PASTE Variable Val in A1'!A191</f>
         <v>AAPIORIGIN_OTHERPACIFICISLANDER</v>
@@ -6473,7 +6503,7 @@
         <v>No</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C191" s="4">
         <f>'[1]PASTE Variable Val in A1'!B192</f>
         <v>1</v>
@@ -6483,7 +6513,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A192" t="str">
         <f>'[1]PASTE Variable Val in A1'!A193</f>
         <v>AAPIORIGIN_OTHERAAPIORIGIN</v>
@@ -6501,7 +6531,7 @@
         <v>No</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C193" s="4">
         <f>'[1]PASTE Variable Val in A1'!B194</f>
         <v>1</v>
@@ -6511,7 +6541,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A194" t="str">
         <f>'[1]PASTE Variable Val in A1'!A195</f>
         <v>LANG_ATHOME</v>
@@ -6529,7 +6559,7 @@
         <v>English</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C195" s="4">
         <f>'[1]PASTE Variable Val in A1'!B196</f>
         <v>2</v>
@@ -6539,7 +6569,7 @@
         <v>Chinese</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C196" s="4">
         <f>'[1]PASTE Variable Val in A1'!B197</f>
         <v>3</v>
@@ -6549,7 +6579,7 @@
         <v>Korean</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C197" s="4">
         <f>'[1]PASTE Variable Val in A1'!B198</f>
         <v>4</v>
@@ -6559,7 +6589,7 @@
         <v>Tagalog</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C198" s="4">
         <f>'[1]PASTE Variable Val in A1'!B199</f>
         <v>5</v>
@@ -6569,7 +6599,7 @@
         <v>Vietnamese</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C199" s="4">
         <f>'[1]PASTE Variable Val in A1'!B200</f>
         <v>6</v>
@@ -6579,7 +6609,7 @@
         <v>Other Language</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C200" s="4">
         <f>'[1]PASTE Variable Val in A1'!B201</f>
         <v>77</v>
@@ -6589,7 +6619,7 @@
         <v>DON'T KNOW</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C201" s="4">
         <f>'[1]PASTE Variable Val in A1'!B202</f>
         <v>98</v>
@@ -6599,7 +6629,7 @@
         <v>SKIPPED ON WEB</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C202" s="4">
         <f>'[1]PASTE Variable Val in A1'!B203</f>
         <v>99</v>
@@ -6609,7 +6639,7 @@
         <v>REFUSED</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A203" t="str">
         <f>'[1]PASTE Variable Val in A1'!A204</f>
         <v>COO</v>
@@ -6627,7 +6657,7 @@
         <v>In the United States</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C204" s="4">
         <f>'[1]PASTE Variable Val in A1'!B205</f>
         <v>2</v>
@@ -6637,7 +6667,7 @@
         <v>Outside the United States</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C205" s="4">
         <f>'[1]PASTE Variable Val in A1'!B206</f>
         <v>77</v>
@@ -6647,7 +6677,7 @@
         <v>DON'T KNOW</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C206" s="4">
         <f>'[1]PASTE Variable Val in A1'!B207</f>
         <v>98</v>
@@ -6657,7 +6687,7 @@
         <v>SKIPPED ON WEB</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C207" s="4">
         <f>'[1]PASTE Variable Val in A1'!B208</f>
         <v>99</v>
@@ -6667,7 +6697,7 @@
         <v>REFUSED</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A208" t="str">
         <f>'[1]PASTE Variable Val in A1'!A209</f>
         <v>FATHER</v>
@@ -6685,7 +6715,7 @@
         <v>In the United States</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C209" s="4">
         <f>'[1]PASTE Variable Val in A1'!B210</f>
         <v>2</v>
@@ -6695,7 +6725,7 @@
         <v>Outside the United States</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C210" s="4">
         <f>'[1]PASTE Variable Val in A1'!B211</f>
         <v>77</v>
@@ -6705,7 +6735,7 @@
         <v>DON'T KNOW</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C211" s="4">
         <f>'[1]PASTE Variable Val in A1'!B212</f>
         <v>98</v>
@@ -6715,7 +6745,7 @@
         <v>SKIPPED ON WEB</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C212" s="4">
         <f>'[1]PASTE Variable Val in A1'!B213</f>
         <v>99</v>
@@ -6725,7 +6755,7 @@
         <v>REFUSED</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A213" t="str">
         <f>'[1]PASTE Variable Val in A1'!A214</f>
         <v>MOTHER</v>
@@ -6743,7 +6773,7 @@
         <v>In the United States</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C214" s="4">
         <f>'[1]PASTE Variable Val in A1'!B215</f>
         <v>2</v>
@@ -6753,7 +6783,7 @@
         <v>Outside the United States</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C215" s="4">
         <f>'[1]PASTE Variable Val in A1'!B216</f>
         <v>77</v>
@@ -6763,7 +6793,7 @@
         <v>DON'T KNOW</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C216" s="4">
         <f>'[1]PASTE Variable Val in A1'!B217</f>
         <v>98</v>
@@ -6773,7 +6803,7 @@
         <v>SKIPPED ON WEB</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C217" s="4">
         <f>'[1]PASTE Variable Val in A1'!B218</f>
         <v>99</v>
@@ -6783,7 +6813,7 @@
         <v>REFUSED</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A218" t="str">
         <f>'[1]PASTE Variable Val in A1'!A219</f>
         <v>EDUC5</v>
@@ -6801,7 +6831,7 @@
         <v>Less than HS</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C219" s="4">
         <f>'[1]PASTE Variable Val in A1'!B220</f>
         <v>2</v>
@@ -6811,7 +6841,7 @@
         <v>HS graduate or equivalent</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C220" s="4">
         <f>'[1]PASTE Variable Val in A1'!B221</f>
         <v>3</v>
@@ -6821,7 +6851,7 @@
         <v>Some college/ associates degree</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C221" s="4">
         <f>'[1]PASTE Variable Val in A1'!B222</f>
         <v>4</v>
@@ -6831,7 +6861,7 @@
         <v>Bachelor's degree</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C222" s="4">
         <f>'[1]PASTE Variable Val in A1'!B223</f>
         <v>5</v>
@@ -6841,7 +6871,7 @@
         <v>Post grad study/professional degree</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A223" t="str">
         <f>'[1]PASTE Variable Val in A1'!A224</f>
         <v>MARITAL</v>
@@ -6859,7 +6889,7 @@
         <v>Married</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C224" s="4">
         <f>'[1]PASTE Variable Val in A1'!B225</f>
         <v>2</v>
@@ -6869,7 +6899,7 @@
         <v>Widowed</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C225" s="4">
         <f>'[1]PASTE Variable Val in A1'!B226</f>
         <v>3</v>
@@ -6879,7 +6909,7 @@
         <v>Divorced</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C226" s="4">
         <f>'[1]PASTE Variable Val in A1'!B227</f>
         <v>4</v>
@@ -6889,7 +6919,7 @@
         <v>Separated</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C227" s="4">
         <f>'[1]PASTE Variable Val in A1'!B228</f>
         <v>5</v>
@@ -6899,7 +6929,7 @@
         <v>Never married</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C228" s="4">
         <f>'[1]PASTE Variable Val in A1'!B229</f>
         <v>6</v>
@@ -6909,7 +6939,7 @@
         <v>Living with partner</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A229" t="str">
         <f>'[1]PASTE Variable Val in A1'!A230</f>
         <v>EMPLOY</v>
@@ -6927,7 +6957,7 @@
         <v>Working - as a paid employee</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C230" s="4">
         <f>'[1]PASTE Variable Val in A1'!B231</f>
         <v>2</v>
@@ -6937,7 +6967,7 @@
         <v>Working - self-employed</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C231" s="4">
         <f>'[1]PASTE Variable Val in A1'!B232</f>
         <v>3</v>
@@ -6947,7 +6977,7 @@
         <v>Not working - on temporary layoff from a job</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C232" s="4">
         <f>'[1]PASTE Variable Val in A1'!B233</f>
         <v>4</v>
@@ -6957,7 +6987,7 @@
         <v>Not working - looking for work</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C233" s="4">
         <f>'[1]PASTE Variable Val in A1'!B234</f>
         <v>5</v>
@@ -6967,7 +6997,7 @@
         <v>Not working - retired</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C234" s="4">
         <f>'[1]PASTE Variable Val in A1'!B235</f>
         <v>6</v>
@@ -6977,7 +7007,7 @@
         <v>Not working - disabled</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C235" s="4">
         <f>'[1]PASTE Variable Val in A1'!B236</f>
         <v>7</v>
@@ -6987,7 +7017,7 @@
         <v>Not working - other</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A236" t="str">
         <f>'[1]PASTE Variable Val in A1'!A237</f>
         <v>INCOME</v>
@@ -7005,7 +7035,7 @@
         <v>Less than $5,000</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C237" s="4">
         <f>'[1]PASTE Variable Val in A1'!B238</f>
         <v>2</v>
@@ -7015,7 +7045,7 @@
         <v>$5,000 to $9,999</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C238" s="4">
         <f>'[1]PASTE Variable Val in A1'!B239</f>
         <v>3</v>
@@ -7025,7 +7055,7 @@
         <v>$10,000 to $14,999</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C239" s="4">
         <f>'[1]PASTE Variable Val in A1'!B240</f>
         <v>4</v>
@@ -7035,7 +7065,7 @@
         <v>$15,000 to $19,999</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C240" s="4">
         <f>'[1]PASTE Variable Val in A1'!B241</f>
         <v>5</v>
@@ -7045,7 +7075,7 @@
         <v>$20,000 to $24,999</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C241" s="4">
         <f>'[1]PASTE Variable Val in A1'!B242</f>
         <v>6</v>
@@ -7055,7 +7085,7 @@
         <v>$25,000 to $29,999</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C242" s="4">
         <f>'[1]PASTE Variable Val in A1'!B243</f>
         <v>7</v>
@@ -7065,7 +7095,7 @@
         <v>$30,000 to $34,999</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C243" s="4">
         <f>'[1]PASTE Variable Val in A1'!B244</f>
         <v>8</v>
@@ -7075,7 +7105,7 @@
         <v>$35,000 to $39,999</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C244" s="4">
         <f>'[1]PASTE Variable Val in A1'!B245</f>
         <v>9</v>
@@ -7085,7 +7115,7 @@
         <v>$40,000 to $49,999</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C245" s="4">
         <f>'[1]PASTE Variable Val in A1'!B246</f>
         <v>10</v>
@@ -7095,7 +7125,7 @@
         <v>$50,000 to $59,999</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C246" s="4">
         <f>'[1]PASTE Variable Val in A1'!B247</f>
         <v>11</v>
@@ -7105,7 +7135,7 @@
         <v>$60,000 to $74,999</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C247" s="4">
         <f>'[1]PASTE Variable Val in A1'!B248</f>
         <v>12</v>
@@ -7115,7 +7145,7 @@
         <v>$75,000 to $84,999</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C248" s="4">
         <f>'[1]PASTE Variable Val in A1'!B249</f>
         <v>13</v>
@@ -7125,7 +7155,7 @@
         <v>$85,000 to $99,999</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C249" s="4">
         <f>'[1]PASTE Variable Val in A1'!B250</f>
         <v>14</v>
@@ -7135,7 +7165,7 @@
         <v>$100,000 to $124,999</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C250" s="4">
         <f>'[1]PASTE Variable Val in A1'!B251</f>
         <v>15</v>
@@ -7145,7 +7175,7 @@
         <v>$125,000 to $149,999</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C251" s="4">
         <f>'[1]PASTE Variable Val in A1'!B252</f>
         <v>16</v>
@@ -7155,7 +7185,7 @@
         <v>$150,000 to $174,999</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C252" s="4">
         <f>'[1]PASTE Variable Val in A1'!B253</f>
         <v>17</v>
@@ -7165,7 +7195,7 @@
         <v>$175,000 to $199,999</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C253" s="4">
         <f>'[1]PASTE Variable Val in A1'!B254</f>
         <v>18</v>
@@ -7175,7 +7205,7 @@
         <v>$200,000 or more</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A254" t="str">
         <f>'[1]PASTE Variable Val in A1'!A255</f>
         <v>INCOME4</v>
@@ -7193,7 +7223,7 @@
         <v>Less than $30,000</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C255" s="4">
         <f>'[1]PASTE Variable Val in A1'!B256</f>
         <v>2</v>
@@ -7203,7 +7233,7 @@
         <v>$30,000 to under $60,000</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C256" s="4">
         <f>'[1]PASTE Variable Val in A1'!B257</f>
         <v>3</v>
@@ -7213,7 +7243,7 @@
         <v>$60,000 to under $100,000</v>
       </c>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C257" s="4">
         <f>'[1]PASTE Variable Val in A1'!B258</f>
         <v>4</v>
@@ -7223,7 +7253,7 @@
         <v>$100,000 or more</v>
       </c>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A258" t="str">
         <f>'[1]PASTE Variable Val in A1'!A259</f>
         <v>INCOME9</v>
@@ -7241,7 +7271,7 @@
         <v>Under $10,000</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C259" s="4">
         <f>'[1]PASTE Variable Val in A1'!B260</f>
         <v>2</v>
@@ -7251,7 +7281,7 @@
         <v>$10,000 to under $20,000</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C260" s="4">
         <f>'[1]PASTE Variable Val in A1'!B261</f>
         <v>3</v>
@@ -7261,7 +7291,7 @@
         <v>$20,000 to under $30,000</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C261" s="4">
         <f>'[1]PASTE Variable Val in A1'!B262</f>
         <v>4</v>
@@ -7271,7 +7301,7 @@
         <v>$30,000 to under $40,000</v>
       </c>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C262" s="4">
         <f>'[1]PASTE Variable Val in A1'!B263</f>
         <v>5</v>
@@ -7281,7 +7311,7 @@
         <v>$40,000 to under $50,000</v>
       </c>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C263" s="4">
         <f>'[1]PASTE Variable Val in A1'!B264</f>
         <v>6</v>
@@ -7291,7 +7321,7 @@
         <v>$50,000 to under $75,000</v>
       </c>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C264" s="4">
         <f>'[1]PASTE Variable Val in A1'!B265</f>
         <v>7</v>
@@ -7301,7 +7331,7 @@
         <v>$75,000 to under $100,000</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C265" s="4">
         <f>'[1]PASTE Variable Val in A1'!B266</f>
         <v>8</v>
@@ -7311,7 +7341,7 @@
         <v>$100,000 to under $150,000</v>
       </c>
     </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C266" s="4">
         <f>'[1]PASTE Variable Val in A1'!B267</f>
         <v>9</v>
@@ -7321,7 +7351,7 @@
         <v>$150,000 or more</v>
       </c>
     </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A267" t="str">
         <f>'[1]PASTE Variable Val in A1'!A268</f>
         <v>STATE</v>
@@ -7339,7 +7369,7 @@
         <v>DON'T KNOW</v>
       </c>
     </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C268" s="4">
         <f>'[1]PASTE Variable Val in A1'!B269</f>
         <v>99</v>
@@ -7349,7 +7379,7 @@
         <v>REFUSED</v>
       </c>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C269" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B270</f>
         <v>AK</v>
@@ -7359,7 +7389,7 @@
         <v>Alaska</v>
       </c>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C270" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B271</f>
         <v>AL</v>
@@ -7369,7 +7399,7 @@
         <v>Alabama</v>
       </c>
     </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C271" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B272</f>
         <v>AR</v>
@@ -7379,7 +7409,7 @@
         <v>Arkansas</v>
       </c>
     </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C272" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B273</f>
         <v>AZ</v>
@@ -7389,7 +7419,7 @@
         <v>Arizona</v>
       </c>
     </row>
-    <row r="273" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="273" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C273" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B274</f>
         <v>CA</v>
@@ -7399,7 +7429,7 @@
         <v>California</v>
       </c>
     </row>
-    <row r="274" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="274" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C274" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B275</f>
         <v>CO</v>
@@ -7409,7 +7439,7 @@
         <v>Colorado</v>
       </c>
     </row>
-    <row r="275" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="275" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C275" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B276</f>
         <v>CT</v>
@@ -7419,7 +7449,7 @@
         <v>Connecticut</v>
       </c>
     </row>
-    <row r="276" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="276" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C276" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B277</f>
         <v>DC</v>
@@ -7429,7 +7459,7 @@
         <v>District of Columbia</v>
       </c>
     </row>
-    <row r="277" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="277" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C277" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B278</f>
         <v>DE</v>
@@ -7439,7 +7469,7 @@
         <v>Delaware</v>
       </c>
     </row>
-    <row r="278" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="278" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C278" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B279</f>
         <v>FL</v>
@@ -7449,7 +7479,7 @@
         <v>Florida</v>
       </c>
     </row>
-    <row r="279" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="279" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C279" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B280</f>
         <v>GA</v>
@@ -7459,7 +7489,7 @@
         <v>Georgia</v>
       </c>
     </row>
-    <row r="280" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="280" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C280" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B281</f>
         <v>HI</v>
@@ -7469,7 +7499,7 @@
         <v>Hawaii</v>
       </c>
     </row>
-    <row r="281" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="281" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C281" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B282</f>
         <v>IA</v>
@@ -7479,7 +7509,7 @@
         <v>Iowa</v>
       </c>
     </row>
-    <row r="282" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="282" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C282" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B283</f>
         <v>ID</v>
@@ -7489,7 +7519,7 @@
         <v>Idaho</v>
       </c>
     </row>
-    <row r="283" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="283" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C283" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B284</f>
         <v>IL</v>
@@ -7499,7 +7529,7 @@
         <v>Illinois</v>
       </c>
     </row>
-    <row r="284" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="284" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C284" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B285</f>
         <v>IN</v>
@@ -7509,7 +7539,7 @@
         <v>Indiana</v>
       </c>
     </row>
-    <row r="285" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="285" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C285" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B286</f>
         <v>KS</v>
@@ -7519,7 +7549,7 @@
         <v>Kansas</v>
       </c>
     </row>
-    <row r="286" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="286" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C286" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B287</f>
         <v>KY</v>
@@ -7529,7 +7559,7 @@
         <v>Kentucky</v>
       </c>
     </row>
-    <row r="287" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="287" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C287" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B288</f>
         <v>LA</v>
@@ -7539,7 +7569,7 @@
         <v>Louisiana</v>
       </c>
     </row>
-    <row r="288" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="288" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C288" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B289</f>
         <v>MA</v>
@@ -7549,7 +7579,7 @@
         <v>Massachusetts</v>
       </c>
     </row>
-    <row r="289" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="289" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C289" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B290</f>
         <v>MD</v>
@@ -7559,7 +7589,7 @@
         <v>Maryland</v>
       </c>
     </row>
-    <row r="290" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="290" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C290" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B291</f>
         <v>ME</v>
@@ -7569,7 +7599,7 @@
         <v>Maine</v>
       </c>
     </row>
-    <row r="291" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="291" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C291" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B292</f>
         <v>MI</v>
@@ -7579,7 +7609,7 @@
         <v>Michigan</v>
       </c>
     </row>
-    <row r="292" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="292" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C292" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B293</f>
         <v>MN</v>
@@ -7589,7 +7619,7 @@
         <v>Minnesota</v>
       </c>
     </row>
-    <row r="293" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="293" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C293" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B294</f>
         <v>MO</v>
@@ -7599,7 +7629,7 @@
         <v>Missouri</v>
       </c>
     </row>
-    <row r="294" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="294" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C294" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B295</f>
         <v>MS</v>
@@ -7609,7 +7639,7 @@
         <v>Mississippi</v>
       </c>
     </row>
-    <row r="295" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="295" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C295" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B296</f>
         <v>MT</v>
@@ -7619,7 +7649,7 @@
         <v>Montana</v>
       </c>
     </row>
-    <row r="296" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="296" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C296" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B297</f>
         <v>NC</v>
@@ -7629,7 +7659,7 @@
         <v>North Carolina</v>
       </c>
     </row>
-    <row r="297" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="297" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C297" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B298</f>
         <v>ND</v>
@@ -7639,7 +7669,7 @@
         <v>North Dakota</v>
       </c>
     </row>
-    <row r="298" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="298" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C298" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B299</f>
         <v>NE</v>
@@ -7649,7 +7679,7 @@
         <v>Nebraska</v>
       </c>
     </row>
-    <row r="299" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="299" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C299" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B300</f>
         <v>NH</v>
@@ -7659,7 +7689,7 @@
         <v>New Hampshire</v>
       </c>
     </row>
-    <row r="300" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="300" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C300" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B301</f>
         <v>NJ</v>
@@ -7669,7 +7699,7 @@
         <v>New Jersey</v>
       </c>
     </row>
-    <row r="301" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="301" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C301" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B302</f>
         <v>NM</v>
@@ -7679,7 +7709,7 @@
         <v>New Mexico</v>
       </c>
     </row>
-    <row r="302" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="302" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C302" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B303</f>
         <v>NV</v>
@@ -7689,7 +7719,7 @@
         <v>Nevada</v>
       </c>
     </row>
-    <row r="303" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="303" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C303" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B304</f>
         <v>NY</v>
@@ -7699,7 +7729,7 @@
         <v>New York</v>
       </c>
     </row>
-    <row r="304" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="304" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C304" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B305</f>
         <v>OH</v>
@@ -7709,7 +7739,7 @@
         <v>Ohio</v>
       </c>
     </row>
-    <row r="305" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="305" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C305" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B306</f>
         <v>OK</v>
@@ -7719,7 +7749,7 @@
         <v>Oklahoma</v>
       </c>
     </row>
-    <row r="306" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="306" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C306" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B307</f>
         <v>OR</v>
@@ -7729,7 +7759,7 @@
         <v>Oregon</v>
       </c>
     </row>
-    <row r="307" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="307" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C307" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B308</f>
         <v>PA</v>
@@ -7739,7 +7769,7 @@
         <v>Pennsylvania</v>
       </c>
     </row>
-    <row r="308" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="308" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C308" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B309</f>
         <v>RI</v>
@@ -7749,7 +7779,7 @@
         <v>Rhode Island</v>
       </c>
     </row>
-    <row r="309" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="309" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C309" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B310</f>
         <v>SC</v>
@@ -7759,7 +7789,7 @@
         <v>South Carolina</v>
       </c>
     </row>
-    <row r="310" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="310" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C310" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B311</f>
         <v>SD</v>
@@ -7769,7 +7799,7 @@
         <v>South Dakota</v>
       </c>
     </row>
-    <row r="311" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="311" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C311" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B312</f>
         <v>TN</v>
@@ -7779,7 +7809,7 @@
         <v>Tennessee</v>
       </c>
     </row>
-    <row r="312" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="312" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C312" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B313</f>
         <v>TX</v>
@@ -7789,7 +7819,7 @@
         <v>Texas</v>
       </c>
     </row>
-    <row r="313" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="313" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C313" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B314</f>
         <v>UT</v>
@@ -7799,7 +7829,7 @@
         <v>Utah</v>
       </c>
     </row>
-    <row r="314" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="314" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C314" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B315</f>
         <v>VA</v>
@@ -7809,7 +7839,7 @@
         <v>Virginia</v>
       </c>
     </row>
-    <row r="315" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="315" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C315" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B316</f>
         <v>VI</v>
@@ -7819,7 +7849,7 @@
         <v>Virgin Islands</v>
       </c>
     </row>
-    <row r="316" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="316" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C316" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B317</f>
         <v>VT</v>
@@ -7829,7 +7859,7 @@
         <v>Vermont</v>
       </c>
     </row>
-    <row r="317" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="317" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C317" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B318</f>
         <v>WA</v>
@@ -7839,7 +7869,7 @@
         <v>Washington</v>
       </c>
     </row>
-    <row r="318" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="318" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C318" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B319</f>
         <v>WI</v>
@@ -7849,7 +7879,7 @@
         <v>Wisconsin</v>
       </c>
     </row>
-    <row r="319" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="319" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C319" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B320</f>
         <v>WV</v>
@@ -7859,7 +7889,7 @@
         <v>West Virginia</v>
       </c>
     </row>
-    <row r="320" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="320" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C320" s="4" t="str">
         <f>'[1]PASTE Variable Val in A1'!B321</f>
         <v>WY</v>
@@ -7869,7 +7899,7 @@
         <v>Wyoming</v>
       </c>
     </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A321" t="str">
         <f>'[1]PASTE Variable Val in A1'!A322</f>
         <v>REGION4</v>
@@ -7887,7 +7917,7 @@
         <v>Northeast</v>
       </c>
     </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C322" s="4">
         <f>'[1]PASTE Variable Val in A1'!B323</f>
         <v>2</v>
@@ -7897,7 +7927,7 @@
         <v>Midwest</v>
       </c>
     </row>
-    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C323" s="4">
         <f>'[1]PASTE Variable Val in A1'!B324</f>
         <v>3</v>
@@ -7907,7 +7937,7 @@
         <v>South</v>
       </c>
     </row>
-    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C324" s="4">
         <f>'[1]PASTE Variable Val in A1'!B325</f>
         <v>4</v>
@@ -7917,7 +7947,7 @@
         <v>West</v>
       </c>
     </row>
-    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A325" t="str">
         <f>'[1]PASTE Variable Val in A1'!A326</f>
         <v>REGION9</v>
@@ -7935,7 +7965,7 @@
         <v>New England</v>
       </c>
     </row>
-    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C326" s="4">
         <f>'[1]PASTE Variable Val in A1'!B327</f>
         <v>2</v>
@@ -7945,7 +7975,7 @@
         <v>Mid-Atlantic</v>
       </c>
     </row>
-    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C327" s="4">
         <f>'[1]PASTE Variable Val in A1'!B328</f>
         <v>3</v>
@@ -7955,7 +7985,7 @@
         <v>East North Central</v>
       </c>
     </row>
-    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C328" s="4">
         <f>'[1]PASTE Variable Val in A1'!B329</f>
         <v>4</v>
@@ -7965,7 +7995,7 @@
         <v>West North Central</v>
       </c>
     </row>
-    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C329" s="4">
         <f>'[1]PASTE Variable Val in A1'!B330</f>
         <v>5</v>
@@ -7975,7 +8005,7 @@
         <v>South Atlantic</v>
       </c>
     </row>
-    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C330" s="4">
         <f>'[1]PASTE Variable Val in A1'!B331</f>
         <v>6</v>
@@ -7985,7 +8015,7 @@
         <v>East South Central</v>
       </c>
     </row>
-    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C331" s="4">
         <f>'[1]PASTE Variable Val in A1'!B332</f>
         <v>7</v>
@@ -7995,7 +8025,7 @@
         <v>West South Central</v>
       </c>
     </row>
-    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C332" s="4">
         <f>'[1]PASTE Variable Val in A1'!B333</f>
         <v>8</v>
@@ -8005,7 +8035,7 @@
         <v>Mountain</v>
       </c>
     </row>
-    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C333" s="4">
         <f>'[1]PASTE Variable Val in A1'!B334</f>
         <v>9</v>
@@ -8015,7 +8045,7 @@
         <v>Pacific</v>
       </c>
     </row>
-    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A334" t="str">
         <f>'[1]PASTE Variable Val in A1'!A335</f>
         <v>METRO</v>
@@ -8033,7 +8063,7 @@
         <v>Non-Metro Area</v>
       </c>
     </row>
-    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C335" s="4">
         <f>'[1]PASTE Variable Val in A1'!B336</f>
         <v>1</v>
@@ -8043,7 +8073,7 @@
         <v>Metro Area</v>
       </c>
     </row>
-    <row r="336" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A336" t="str">
         <f>'[1]PASTE Variable Val in A1'!A337</f>
         <v>INTERNET</v>
@@ -8061,7 +8091,7 @@
         <v>Non-internet household</v>
       </c>
     </row>
-    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C337" s="4">
         <f>'[1]PASTE Variable Val in A1'!B338</f>
         <v>1</v>
@@ -8071,7 +8101,7 @@
         <v>Internet Household</v>
       </c>
     </row>
-    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A338" t="str">
         <f>'[1]PASTE Variable Val in A1'!A339</f>
         <v>HOUSING</v>
@@ -8089,7 +8119,7 @@
         <v>Owned or being bought by you or someone in your household</v>
       </c>
     </row>
-    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C339" s="4">
         <f>'[1]PASTE Variable Val in A1'!B340</f>
         <v>2</v>
@@ -8099,7 +8129,7 @@
         <v>Rented for cash</v>
       </c>
     </row>
-    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C340" s="4">
         <f>'[1]PASTE Variable Val in A1'!B341</f>
         <v>3</v>
@@ -8109,7 +8139,7 @@
         <v>Occupied without payment of cash rent</v>
       </c>
     </row>
-    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A341" t="str">
         <f>'[1]PASTE Variable Val in A1'!A342</f>
         <v>HOME_TYPE</v>
@@ -8127,7 +8157,7 @@
         <v>A one-family house detached from any other house</v>
       </c>
     </row>
-    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C342" s="4">
         <f>'[1]PASTE Variable Val in A1'!B343</f>
         <v>2</v>
@@ -8137,7 +8167,7 @@
         <v>A one-family house attached to one or more houses</v>
       </c>
     </row>
-    <row r="343" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C343" s="4">
         <f>'[1]PASTE Variable Val in A1'!B344</f>
         <v>3</v>
@@ -8147,7 +8177,7 @@
         <v>A building with 2 or more apartments</v>
       </c>
     </row>
-    <row r="344" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C344" s="4">
         <f>'[1]PASTE Variable Val in A1'!B345</f>
         <v>4</v>
@@ -8157,7 +8187,7 @@
         <v>A mobile home or trailer</v>
       </c>
     </row>
-    <row r="345" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C345" s="4">
         <f>'[1]PASTE Variable Val in A1'!B346</f>
         <v>5</v>
@@ -8167,7 +8197,7 @@
         <v>Boat, RV, van, etc</v>
       </c>
     </row>
-    <row r="346" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A346" t="str">
         <f>'[1]PASTE Variable Val in A1'!A347</f>
         <v>PHONESERVICE</v>
@@ -8185,7 +8215,7 @@
         <v>Landline telephone only</v>
       </c>
     </row>
-    <row r="347" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C347" s="4">
         <f>'[1]PASTE Variable Val in A1'!B348</f>
         <v>2</v>
@@ -8195,7 +8225,7 @@
         <v>Have a landline, but mostly use cellphone</v>
       </c>
     </row>
-    <row r="348" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C348" s="4">
         <f>'[1]PASTE Variable Val in A1'!B349</f>
         <v>3</v>
@@ -8205,7 +8235,7 @@
         <v>Have cellphone, but mostly use landline</v>
       </c>
     </row>
-    <row r="349" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C349" s="4">
         <f>'[1]PASTE Variable Val in A1'!B350</f>
         <v>4</v>
@@ -8215,7 +8245,7 @@
         <v>Cellphone only</v>
       </c>
     </row>
-    <row r="350" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C350" s="4">
         <f>'[1]PASTE Variable Val in A1'!B351</f>
         <v>5</v>
@@ -8225,7 +8255,7 @@
         <v>No telephone service</v>
       </c>
     </row>
-    <row r="351" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A351" t="str">
         <f>'[1]PASTE Variable Val in A1'!A352</f>
         <v>HHSIZE</v>
@@ -8243,7 +8273,7 @@
         <v>One person, I live by myself</v>
       </c>
     </row>
-    <row r="352" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C352" s="4">
         <f>'[1]PASTE Variable Val in A1'!B353</f>
         <v>2</v>
@@ -8253,7 +8283,7 @@
         <v>Two persons</v>
       </c>
     </row>
-    <row r="353" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="353" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C353" s="4">
         <f>'[1]PASTE Variable Val in A1'!B354</f>
         <v>3</v>
@@ -8263,7 +8293,7 @@
         <v>Three persons</v>
       </c>
     </row>
-    <row r="354" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="354" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C354" s="4">
         <f>'[1]PASTE Variable Val in A1'!B355</f>
         <v>4</v>
@@ -8273,7 +8303,7 @@
         <v>Four persons</v>
       </c>
     </row>
-    <row r="355" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="355" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C355" s="4">
         <f>'[1]PASTE Variable Val in A1'!B356</f>
         <v>5</v>
@@ -8283,7 +8313,7 @@
         <v>Five persons</v>
       </c>
     </row>
-    <row r="356" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="356" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C356" s="4">
         <f>'[1]PASTE Variable Val in A1'!B357</f>
         <v>6</v>

</xml_diff>